<commit_message>
update al correo automatizado
Se actualiza el saludo del correo automático
</commit_message>
<xml_diff>
--- a/correos/correos_prueba.xlsx
+++ b/correos/correos_prueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educacionpublica-my.sharepoint.com/personal/alonso_arrano_dep_cl/Documents/2024/SAE - Anotate en la lista/reporteria_ael/correos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="11_AD4D2F04E46CFB4ACB3E20CA8550FF6C693EDF25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{931D33D5-1393-4960-9B92-1EE19A7DC0CE}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="11_AD4D2F04E46CFB4ACB3E20CA8550FF6C693EDF25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D037D37F-3368-4CEC-BB01-0DBD5F3EE8C0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5595" yWindow="225" windowWidth="14400" windowHeight="7350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="147">
   <si>
     <t>SLEP</t>
   </si>
@@ -459,9 +459,6 @@
     <t>claudio.wilson@sleplosalamos.gob.cl</t>
   </si>
   <si>
-    <t>reporte_petroca.html</t>
-  </si>
-  <si>
     <t>reporte_los_andes.html</t>
   </si>
   <si>
@@ -472,6 +469,18 @@
   </si>
   <si>
     <t>reporte_los_álamos.html</t>
+  </si>
+  <si>
+    <t>Genero</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>reporte_petorca.html</t>
   </si>
 </sst>
 </file>
@@ -555,19 +564,19 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -576,10 +585,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -587,18 +596,86 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="20">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray125">
+          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -685,6 +762,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -712,84 +809,16 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -805,19 +834,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB655D7C-9877-46E0-92DF-E3EBF603DAAC}" name="Tabla1" displayName="Tabla1" ref="A1:H34" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="A1:H34" xr:uid="{FB655D7C-9877-46E0-92DF-E3EBF603DAAC}"/>
-  <tableColumns count="8">
-    <tableColumn id="7" xr3:uid="{81F1FDBA-6F8D-4F84-B350-BE6DAEB4513E}" name="Tipo_SLEP" dataDxfId="8"/>
-    <tableColumn id="1" xr3:uid="{71E197A0-A7D1-4117-A637-141CAE5153C7}" name="SLEP" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{7E154C76-62D9-49AC-8A5C-38CF45CFD1DA}" name="Nombre Completo" dataDxfId="6" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="6" xr3:uid="{B28C7421-A9F8-41E9-9CE2-9190783BC6C3}" name="Nombre" dataDxfId="5" dataCellStyle="Hipervínculo">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FB655D7C-9877-46E0-92DF-E3EBF603DAAC}" name="Tabla1" displayName="Tabla1" ref="A1:I34" totalsRowShown="0" dataDxfId="19">
+  <autoFilter ref="A1:I34" xr:uid="{FB655D7C-9877-46E0-92DF-E3EBF603DAAC}"/>
+  <tableColumns count="9">
+    <tableColumn id="7" xr3:uid="{81F1FDBA-6F8D-4F84-B350-BE6DAEB4513E}" name="Tipo_SLEP" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{71E197A0-A7D1-4117-A637-141CAE5153C7}" name="SLEP" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{7E154C76-62D9-49AC-8A5C-38CF45CFD1DA}" name="Nombre Completo" dataDxfId="16" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="6" xr3:uid="{B28C7421-A9F8-41E9-9CE2-9190783BC6C3}" name="Nombre" dataDxfId="15" dataCellStyle="Hipervínculo">
       <calculatedColumnFormula>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{D31AB802-9D0A-47E2-B51A-3E1504C462E0}" name="RUT" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{BFEBADF9-4E36-4F51-BFFE-B6A3E1E4CDC8}" name="correo" dataDxfId="3" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="4" xr3:uid="{146F0A02-05F8-4FED-86F3-F5493953AC21}" name="copia" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{6F51BF54-5EDB-4B9D-B425-9871551CED2D}" name="archivo" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{9E5CEF83-8F1C-47D8-9D60-176E8AC3FEA4}" name="Genero" dataDxfId="14" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="8" xr3:uid="{D31AB802-9D0A-47E2-B51A-3E1504C462E0}" name="RUT" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{BFEBADF9-4E36-4F51-BFFE-B6A3E1E4CDC8}" name="correo" dataDxfId="12" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="4" xr3:uid="{146F0A02-05F8-4FED-86F3-F5493953AC21}" name="copia" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{6F51BF54-5EDB-4B9D-B425-9871551CED2D}" name="archivo" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1086,24 +1116,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="40.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.26953125" customWidth="1"/>
-    <col min="8" max="8" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -1117,19 +1147,22 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" t="s">
         <v>122</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
@@ -1143,16 +1176,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Ana</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>117</v>
       </c>
@@ -1166,18 +1202,21 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Eduardo</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>117</v>
       </c>
@@ -1191,16 +1230,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Jasmín</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4" t="s">
+      <c r="E4" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>117</v>
       </c>
@@ -1214,18 +1256,21 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Jenson</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4" t="s">
+      <c r="E5" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>117</v>
       </c>
@@ -1239,16 +1284,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Juan</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4" t="s">
+      <c r="E6" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>117</v>
       </c>
@@ -1262,16 +1310,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Yolanda</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="4" t="s">
+      <c r="E7" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>117</v>
       </c>
@@ -1285,16 +1336,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Manuel</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="4" t="s">
+      <c r="E8" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>117</v>
       </c>
@@ -1308,16 +1362,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>David</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="4" t="s">
+      <c r="E9" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="1"/>
+      <c r="I9" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>117</v>
       </c>
@@ -1331,16 +1388,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Marcela</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="4" t="s">
+      <c r="E10" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="1"/>
+      <c r="I10" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>117</v>
       </c>
@@ -1354,16 +1414,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Rodrigo</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="4" t="s">
+      <c r="E11" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>117</v>
       </c>
@@ -1377,18 +1440,21 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Eugenio</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="4" t="s">
+      <c r="E12" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>117</v>
       </c>
@@ -1402,16 +1468,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Carolina</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="4" t="s">
+      <c r="E13" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="1"/>
+      <c r="I13" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>117</v>
       </c>
@@ -1425,18 +1494,21 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Ivy</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="4" t="s">
+      <c r="E14" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>117</v>
       </c>
@@ -1450,16 +1522,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Mario</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="4" t="s">
+      <c r="E15" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="1"/>
+      <c r="I15" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>117</v>
       </c>
@@ -1473,16 +1548,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Sandra</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="4" t="s">
+      <c r="E16" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="1"/>
+      <c r="I16" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>117</v>
       </c>
@@ -1496,16 +1574,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Marcelo</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="4" t="s">
+      <c r="E17" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="1"/>
+      <c r="I17" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>117</v>
       </c>
@@ -1519,16 +1600,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Maryorie</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="4" t="s">
+      <c r="E18" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="1"/>
+      <c r="I18" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>117</v>
       </c>
@@ -1542,16 +1626,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Margarita</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="4" t="s">
+      <c r="E19" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="1"/>
+      <c r="I19" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>117</v>
       </c>
@@ -1565,16 +1652,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Angeline</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="4" t="s">
+      <c r="E20" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="1"/>
+      <c r="I20" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>117</v>
       </c>
@@ -1588,16 +1678,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Daniela</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="4" t="s">
+      <c r="E21" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
+      <c r="H21" s="1"/>
+      <c r="I21" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>117</v>
       </c>
@@ -1611,16 +1704,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Marta</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="4" t="s">
+      <c r="E22" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="1"/>
+      <c r="I22" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>117</v>
       </c>
@@ -1634,16 +1730,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Oscar</v>
       </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="4" t="s">
+      <c r="E23" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
+      <c r="H23" s="1"/>
+      <c r="I23" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>117</v>
       </c>
@@ -1657,16 +1756,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Elena</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="4" t="s">
+      <c r="E24" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="1"/>
+      <c r="I24" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>117</v>
       </c>
@@ -1680,18 +1782,21 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Carolina</v>
       </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="4" t="s">
+      <c r="E25" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>117</v>
       </c>
@@ -1705,16 +1810,19 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Tomás</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="4" t="s">
+      <c r="E26" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1" t="s">
+      <c r="H26" s="1"/>
+      <c r="I26" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>117</v>
       </c>
@@ -1728,18 +1836,21 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Rosita</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="4" t="s">
+      <c r="E27" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>118</v>
       </c>
@@ -1753,18 +1864,21 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Carolina</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="G28" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="H28" s="1"/>
+      <c r="I28" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>118</v>
       </c>
@@ -1778,18 +1892,21 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Miguel</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="G29" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="H29" s="1"/>
+      <c r="I29" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>118</v>
       </c>
@@ -1803,18 +1920,21 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Claudia</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="G30" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.35">
+      <c r="H30" s="1"/>
+      <c r="I30" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>118</v>
       </c>
@@ -1828,18 +1948,21 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Javiera</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F31" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="G31" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H31" s="1"/>
+      <c r="I31" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>118</v>
       </c>
@@ -1853,113 +1976,118 @@
         <f>LEFT(Tabla1[[#This Row],[Nombre Completo]],SEARCH(" ",Tabla1[[#This Row],[Nombre Completo]],1)-1)</f>
         <v>Claudio</v>
       </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="4" t="s">
+      <c r="E32" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H32" s="1"/>
+      <c r="I32" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="6"/>
       <c r="D33" s="7"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="1"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="4"/>
       <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="6"/>
       <c r="D34" s="7"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="1"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="4"/>
       <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:B3">
-    <cfRule type="expression" dxfId="18" priority="19">
-      <formula>$U3=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:F4 B5:E5 G5 G14 A4:A5 A14:E14">
-    <cfRule type="expression" dxfId="17" priority="18">
-      <formula>$T4=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6:F13">
-    <cfRule type="expression" dxfId="16" priority="9">
-      <formula>$T6=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:F25">
-    <cfRule type="expression" dxfId="15" priority="4">
-      <formula>$T15=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:E2">
-    <cfRule type="expression" dxfId="14" priority="21">
-      <formula>$U2=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="expression" dxfId="13" priority="16">
-      <formula>$T5=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:G2">
-    <cfRule type="expression" dxfId="12" priority="20">
-      <formula>$U2=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G25">
-    <cfRule type="expression" dxfId="11" priority="3">
-      <formula>$T25=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A6:A13">
-    <cfRule type="expression" dxfId="10" priority="2">
-      <formula>$T6=1</formula>
+  <conditionalFormatting sqref="A4:A13 B5:F5 H5 A14:F14 H14">
+    <cfRule type="expression" dxfId="9" priority="2">
+      <formula>$U4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:A25">
-    <cfRule type="expression" dxfId="9" priority="1">
-      <formula>$T15=1</formula>
+    <cfRule type="expression" dxfId="8" priority="1">
+      <formula>$U15=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:B3">
+    <cfRule type="expression" dxfId="7" priority="19">
+      <formula>$V3=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:G4">
+    <cfRule type="expression" dxfId="6" priority="18">
+      <formula>$U4=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:G13">
+    <cfRule type="expression" dxfId="5" priority="9">
+      <formula>$U6=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:G25">
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>$U15=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:F2">
+    <cfRule type="expression" dxfId="3" priority="21">
+      <formula>$V2=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="expression" dxfId="2" priority="16">
+      <formula>$U5=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:H2">
+    <cfRule type="expression" dxfId="1" priority="20">
+      <formula>$V2=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25">
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>$U25=1</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{C0737CE7-E542-4D1C-BA03-6991C3CF34C6}"/>
-    <hyperlink ref="G3" r:id="rId2" display="luis.gajardo@slepchiloe.gob.cl;" xr:uid="{8687092E-077F-44E0-8596-381E03D641E8}"/>
-    <hyperlink ref="F6" r:id="rId3" xr:uid="{00B2325A-F588-41ED-AC5B-9DB5D89931CC}"/>
-    <hyperlink ref="F9" r:id="rId4" xr:uid="{13C55916-204E-4C3E-A397-C0E811E2FDC2}"/>
-    <hyperlink ref="F11" r:id="rId5" xr:uid="{20C85ACE-7FF3-4FE2-BC88-162377C43342}"/>
-    <hyperlink ref="F12" r:id="rId6" xr:uid="{BB5038CA-BC9D-4D65-B196-5820788BA999}"/>
-    <hyperlink ref="G12" r:id="rId7" display="mailto:karla.sepulveda@sleppunillacordillera.cl" xr:uid="{FA9727FC-D1CA-4EF4-B723-4BF30F5C5E51}"/>
-    <hyperlink ref="F13" r:id="rId8" xr:uid="{0773547D-CCAE-4E00-A502-AB5D3C7A5D4F}"/>
-    <hyperlink ref="G14" r:id="rId9" xr:uid="{AC730A02-E5F5-4866-BC84-CA9DE3712292}"/>
-    <hyperlink ref="F14" r:id="rId10" xr:uid="{7231EF4D-AE48-4627-B0B7-6060424EA064}"/>
-    <hyperlink ref="F15" r:id="rId11" xr:uid="{CE4BA5E9-B40D-408E-A689-CDF23E66341C}"/>
-    <hyperlink ref="F16" r:id="rId12" xr:uid="{AEDEA0EB-604C-4C31-9304-42A01F8A5A3D}"/>
-    <hyperlink ref="F18" r:id="rId13" xr:uid="{F7398C85-77F6-4B2F-90F2-2305F57C2050}"/>
-    <hyperlink ref="F17" r:id="rId14" xr:uid="{5716803F-2B2A-4A17-BB69-8FDFE706A2AB}"/>
-    <hyperlink ref="F19" r:id="rId15" xr:uid="{E9048617-0AB9-404F-AD37-74E9A485BE30}"/>
-    <hyperlink ref="F20" r:id="rId16" xr:uid="{E454A7F1-60B0-46A2-BCAF-6EE451073594}"/>
-    <hyperlink ref="F21" r:id="rId17" xr:uid="{1127AC0B-364E-4EAD-9D99-A94EA5C42523}"/>
-    <hyperlink ref="F22" r:id="rId18" xr:uid="{898CFB37-C10F-4164-9DC8-B35726F71024}"/>
-    <hyperlink ref="F23" r:id="rId19" xr:uid="{9ECCB776-E8C3-4105-A6F7-2E6F2A184663}"/>
-    <hyperlink ref="F24" r:id="rId20" xr:uid="{4FC5ADBE-181E-43FF-9751-D6D427F0366F}"/>
-    <hyperlink ref="F25" r:id="rId21" xr:uid="{8A1E636A-763E-4FEA-AA46-C17108413427}"/>
-    <hyperlink ref="G25" r:id="rId22" xr:uid="{BC1D1921-7D71-457C-A023-855DF7FD4289}"/>
-    <hyperlink ref="F28" r:id="rId23" display="mailto:carolina.villagra@sleppetorca.gob.cl" xr:uid="{FA5AB3B0-F9E2-45ED-820A-9057AA7CB237}"/>
-    <hyperlink ref="F30" r:id="rId24" display="mailto:claudia.cubillos@slepaconcagua.gob.cl" xr:uid="{BF5D4A03-B565-4290-A323-81DEBCE5CFFB}"/>
-    <hyperlink ref="F31" r:id="rId25" display="mailto:javiera.rivas@sleppuelche.gob.cl" xr:uid="{0BE46A43-B5C0-4B49-A817-F11FCE265D50}"/>
-    <hyperlink ref="F32" r:id="rId26" display="mailto:claudio.wilson@sleplosalamos.gob.cl" xr:uid="{75417199-A8F7-4F2B-95A4-F7A17C2548B4}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{C0737CE7-E542-4D1C-BA03-6991C3CF34C6}"/>
+    <hyperlink ref="H3" r:id="rId2" display="luis.gajardo@slepchiloe.gob.cl;" xr:uid="{8687092E-077F-44E0-8596-381E03D641E8}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{00B2325A-F588-41ED-AC5B-9DB5D89931CC}"/>
+    <hyperlink ref="G9" r:id="rId4" xr:uid="{13C55916-204E-4C3E-A397-C0E811E2FDC2}"/>
+    <hyperlink ref="G11" r:id="rId5" xr:uid="{20C85ACE-7FF3-4FE2-BC88-162377C43342}"/>
+    <hyperlink ref="G12" r:id="rId6" xr:uid="{BB5038CA-BC9D-4D65-B196-5820788BA999}"/>
+    <hyperlink ref="H12" r:id="rId7" display="mailto:karla.sepulveda@sleppunillacordillera.cl" xr:uid="{FA9727FC-D1CA-4EF4-B723-4BF30F5C5E51}"/>
+    <hyperlink ref="G13" r:id="rId8" xr:uid="{0773547D-CCAE-4E00-A502-AB5D3C7A5D4F}"/>
+    <hyperlink ref="H14" r:id="rId9" xr:uid="{AC730A02-E5F5-4866-BC84-CA9DE3712292}"/>
+    <hyperlink ref="G14" r:id="rId10" xr:uid="{7231EF4D-AE48-4627-B0B7-6060424EA064}"/>
+    <hyperlink ref="G15" r:id="rId11" xr:uid="{CE4BA5E9-B40D-408E-A689-CDF23E66341C}"/>
+    <hyperlink ref="G16" r:id="rId12" xr:uid="{AEDEA0EB-604C-4C31-9304-42A01F8A5A3D}"/>
+    <hyperlink ref="G18" r:id="rId13" xr:uid="{F7398C85-77F6-4B2F-90F2-2305F57C2050}"/>
+    <hyperlink ref="G17" r:id="rId14" xr:uid="{5716803F-2B2A-4A17-BB69-8FDFE706A2AB}"/>
+    <hyperlink ref="G19" r:id="rId15" xr:uid="{E9048617-0AB9-404F-AD37-74E9A485BE30}"/>
+    <hyperlink ref="G20" r:id="rId16" xr:uid="{E454A7F1-60B0-46A2-BCAF-6EE451073594}"/>
+    <hyperlink ref="G21" r:id="rId17" xr:uid="{1127AC0B-364E-4EAD-9D99-A94EA5C42523}"/>
+    <hyperlink ref="G22" r:id="rId18" xr:uid="{898CFB37-C10F-4164-9DC8-B35726F71024}"/>
+    <hyperlink ref="G23" r:id="rId19" xr:uid="{9ECCB776-E8C3-4105-A6F7-2E6F2A184663}"/>
+    <hyperlink ref="G24" r:id="rId20" xr:uid="{4FC5ADBE-181E-43FF-9751-D6D427F0366F}"/>
+    <hyperlink ref="G25" r:id="rId21" xr:uid="{8A1E636A-763E-4FEA-AA46-C17108413427}"/>
+    <hyperlink ref="H25" r:id="rId22" xr:uid="{BC1D1921-7D71-457C-A023-855DF7FD4289}"/>
+    <hyperlink ref="G28" r:id="rId23" display="mailto:carolina.villagra@sleppetorca.gob.cl" xr:uid="{FA5AB3B0-F9E2-45ED-820A-9057AA7CB237}"/>
+    <hyperlink ref="G30" r:id="rId24" display="mailto:claudia.cubillos@slepaconcagua.gob.cl" xr:uid="{BF5D4A03-B565-4290-A323-81DEBCE5CFFB}"/>
+    <hyperlink ref="G31" r:id="rId25" display="mailto:javiera.rivas@sleppuelche.gob.cl" xr:uid="{0BE46A43-B5C0-4B49-A817-F11FCE265D50}"/>
+    <hyperlink ref="G32" r:id="rId26" display="mailto:claudio.wilson@sleplosalamos.gob.cl" xr:uid="{75417199-A8F7-4F2B-95A4-F7A17C2548B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1976,134 +2104,134 @@
       <selection sqref="A1:A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>111</v>
       </c>

</xml_diff>